<commit_message>
Update manifest with MCC internal versions
</commit_message>
<xml_diff>
--- a/ManifestDataSource.xlsx
+++ b/ManifestDataSource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\HRDownpatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1084D342-2FD7-4919-B007-E753A6D9B8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848E563-B31F-491C-9103-D18362204564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="3315" windowWidth="31785" windowHeight="16440" xr2:uid="{B9A1D137-BA91-409A-B104-CD27FC2E2057}"/>
+    <workbookView xWindow="2175" yWindow="5805" windowWidth="31785" windowHeight="14895" xr2:uid="{B9A1D137-BA91-409A-B104-CD27FC2E2057}"/>
   </bookViews>
   <sheets>
     <sheet name="Releases" sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3759" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3796" uniqueCount="836">
   <si>
     <t>20 July 2023 – 17:00:58 UTC</t>
   </si>
@@ -2153,15 +2153,6 @@
     <t>MCC_3</t>
   </si>
   <si>
-    <t>MCC Season 9.1</t>
-  </si>
-  <si>
-    <t>MCC Season 9.0</t>
-  </si>
-  <si>
-    <t>MCC Season 9.2</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/11067636381716-Halo-The-Master-Chief-Collection-MCC-Update-December-2022</t>
   </si>
   <si>
@@ -2171,69 +2162,18 @@
     <t>https://support.halowaypoint.com/hc/en-us/articles/17144473706900-Halo-The-Master-Chief-Collection-MCC-Update-July-2023</t>
   </si>
   <si>
-    <t>MCC Season 9.1 Hotfix 2</t>
-  </si>
-  <si>
-    <t>MCC Season 9.2 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 9.1 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/8955559396372-Halo-The-Master-Chief-Collection-MCC-Update-August-2022</t>
   </si>
   <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/5178835359380-Halo-The-Master-Chief-Collection-MCC-Update-April-2022</t>
   </si>
   <si>
-    <t>MCC Season 8.0</t>
-  </si>
-  <si>
-    <t>MCC Season 8.0 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 8.1</t>
-  </si>
-  <si>
-    <t>MCC Season 7.0</t>
-  </si>
-  <si>
-    <t>MCC Season 6.0</t>
-  </si>
-  <si>
-    <t>MCC Season 5.0</t>
-  </si>
-  <si>
-    <t>MCC Season 4.0</t>
-  </si>
-  <si>
-    <t>MCC Season 1.1</t>
-  </si>
-  <si>
-    <t>MCC Season 4.1</t>
-  </si>
-  <si>
-    <t>MCC Season 3.0</t>
-  </si>
-  <si>
-    <t>MCC Season 2.0</t>
-  </si>
-  <si>
-    <t>MCC Season 1.0</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360037688732-Halo-The-Master-Chief-Collection-Patch-Notes-12-18-19</t>
   </si>
   <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360038934552-Halo-The-Master-Chief-Collection-Patch-Notes-1-29-20</t>
   </si>
   <si>
-    <t>MCC Season 1.0 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 1.0 Hotfix 2</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360039995652-Halo-The-Master-Chief-Collection-Patch-Notes-3-3-20</t>
   </si>
   <si>
@@ -2246,30 +2186,18 @@
     <t>MCC/Reach Release</t>
   </si>
   <si>
-    <t>MCC Season 1.1 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360042882732-Halo-The-Master-Chief-Collection-Patch-Notes-5-12-20</t>
   </si>
   <si>
     <t>H2 Release</t>
   </si>
   <si>
-    <t>MCC Season 1.2</t>
-  </si>
-  <si>
-    <t>MCC Season 1.2 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360043511132-Halo-The-Master-Chief-Collection-Patch-Notes-5-21-20</t>
   </si>
   <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360044955912-Halo-The-Master-Chief-Collection-Patch-Notes-6-24-20</t>
   </si>
   <si>
-    <t>MCC Season 1.2 Hotfix 2</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360045689232-Halo-The-Master-Chief-Collection-Patch-Notes-7-14-20</t>
   </si>
   <si>
@@ -2285,27 +2213,18 @@
     <t>https://support.halowaypoint.com/hc/en-us/articles/360046558492-Halo-The-Master-Chief-Collection-Patch-Notes-7-29-20</t>
   </si>
   <si>
-    <t>MCC Season 2.0 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360049316032-Halo-The-Master-Chief-Collection-Patch-Notes-09-22-2020</t>
   </si>
   <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360050949651-Halo-The-Master-Chief-Collection-Patch-Notes-10-14-2020</t>
   </si>
   <si>
-    <t>MCC Season 3.0 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360052057192-Halo-The-Master-Chief-Collection-Patch-Notes-November-2020</t>
   </si>
   <si>
     <t>https://steamdb.info/patchnotes/5702068/</t>
   </si>
   <si>
-    <t>MCC Season 3.0 Hotfix 2</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/360053081732-Halo-The-Master-Chief-Collection-Patch-Notes-December-2020</t>
   </si>
   <si>
@@ -2318,9 +2237,6 @@
     <t>https://support.halowaypoint.com/hc/en-us/articles/360060430971-Halo-The-Master-Chief-Collection-MCC-Patch-Notes-April-2021-CGB-Scale-Test-</t>
   </si>
   <si>
-    <t>MCC Season 6.0 Hotfix 1</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/4402601893268-Halo-The-Master-Chief-Collection-MCC-Patch-Notes-June-2021</t>
   </si>
   <si>
@@ -2330,12 +2246,6 @@
     <t>https://support.halowaypoint.com/hc/en-us/articles/4403514217236-Halo-The-Master-Chief-Collection-MCC-Patch-Notes-July-2021-Hotfix-</t>
   </si>
   <si>
-    <t>MCC Season 7.0 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 7.0 Hotfix 2</t>
-  </si>
-  <si>
     <t>https://support.halowaypoint.com/hc/en-us/articles/4407245081620-Halo-The-Master-Chief-Collection-MCC-Season-8-Patch-Notes-October-2021-</t>
   </si>
   <si>
@@ -2348,27 +2258,9 @@
     <t>https://support.halowaypoint.com/hc/en-us/articles/4411549463316-Halo-The-Master-Chief-Collection-MCC-Hotfix-November-2021</t>
   </si>
   <si>
-    <t>MCC Season 8.1 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 8.2</t>
-  </si>
-  <si>
-    <t>MCC Season 8.2 Hotfix 1</t>
-  </si>
-  <si>
-    <t>MCC Season 8.2 Hotfix 2</t>
-  </si>
-  <si>
-    <t>MCC Season 8.2 Hotfix 3</t>
-  </si>
-  <si>
     <t>https://steamdb.info/patchnotes/8899868/</t>
   </si>
   <si>
-    <t>MCC Season 8.2 Hotfix 4</t>
-  </si>
-  <si>
     <t>https://www.halowaypoint.com/news/welcome-to-reach</t>
   </si>
   <si>
@@ -2445,6 +2337,222 @@
   </si>
   <si>
     <t>Infinite 3</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.3251.0.0</t>
+  </si>
+  <si>
+    <t>1.3232.0.0</t>
+  </si>
+  <si>
+    <t>1.3073.0.0</t>
+  </si>
+  <si>
+    <t>1.3065.0.0</t>
+  </si>
+  <si>
+    <t>1.2969.0.0</t>
+  </si>
+  <si>
+    <t>1.2904.0.0</t>
+  </si>
+  <si>
+    <t>1.2862.0.0</t>
+  </si>
+  <si>
+    <t>1.2845.0.0</t>
+  </si>
+  <si>
+    <t>1.2835.0.0</t>
+  </si>
+  <si>
+    <t>1.2819.0.0</t>
+  </si>
+  <si>
+    <t>1.2645.0.0</t>
+  </si>
+  <si>
+    <t>1.2611.0.0</t>
+  </si>
+  <si>
+    <t>1.2589.0.0</t>
+  </si>
+  <si>
+    <t>1.2580.0.0</t>
+  </si>
+  <si>
+    <t>1.2448.0.0</t>
+  </si>
+  <si>
+    <t>1.2406.0.0</t>
+  </si>
+  <si>
+    <t>1.2398.0.0</t>
+  </si>
+  <si>
+    <t>1.2282.0.0</t>
+  </si>
+  <si>
+    <t>1.2241.0.0</t>
+  </si>
+  <si>
+    <t>1.2094.0.0</t>
+  </si>
+  <si>
+    <t>1.2028.0.0</t>
+  </si>
+  <si>
+    <t>1.1955.0.0</t>
+  </si>
+  <si>
+    <t>1.1871.0.0</t>
+  </si>
+  <si>
+    <t>1.1864.0.0</t>
+  </si>
+  <si>
+    <t>1.1829.0.0</t>
+  </si>
+  <si>
+    <t>1.1716.0.0</t>
+  </si>
+  <si>
+    <t>1.1698.0.0</t>
+  </si>
+  <si>
+    <t>1.1619.0.0</t>
+  </si>
+  <si>
+    <t>1.1570.0.0</t>
+  </si>
+  <si>
+    <t>1.1520.0.0</t>
+  </si>
+  <si>
+    <t>1.1389.0.0</t>
+  </si>
+  <si>
+    <t>1.1384.0.0</t>
+  </si>
+  <si>
+    <t>1.1305.0.0</t>
+  </si>
+  <si>
+    <t>1.1270.0.0</t>
+  </si>
+  <si>
+    <t>1.1246.0.0</t>
+  </si>
+  <si>
+    <t>MCC [1.3251.0.0] Season 9.2 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.3232.0.0] Season 9.2</t>
+  </si>
+  <si>
+    <t>MCC [1.3073.0.0] Season 9.1 Hotfix 2 (Steam Deck EAC Patch)</t>
+  </si>
+  <si>
+    <t>MCC [1.3073.0.0] Season 9.1 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.3065.0.0] Season 9.1</t>
+  </si>
+  <si>
+    <t>MCC [1.2969.0.0] Season 9.0</t>
+  </si>
+  <si>
+    <t>MCC [1.2904.0.0] Season 8.2 Hotfix 4</t>
+  </si>
+  <si>
+    <t>MCC [1.2862.0.0] Season 8.2 Hotfix 3</t>
+  </si>
+  <si>
+    <t>MCC [1.2845.0.0] Season 8.2 Hotfix 2</t>
+  </si>
+  <si>
+    <t>MCC [1.2835.0.0] Season 8.2 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.2819.0.0] Season 8.2</t>
+  </si>
+  <si>
+    <t>MCC [1.2645.0.0] Season 8.1 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.2611.0.0] Season 8.1</t>
+  </si>
+  <si>
+    <t>MCC [1.2589.0.0] Season 8.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.2580.0.0] Season 8.0</t>
+  </si>
+  <si>
+    <t>MCC [1.2448.0.0] Season 7.0 Hotfix 2</t>
+  </si>
+  <si>
+    <t>MCC [1.2406.0.0] Season 7.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.2398.0.0] Season 7.0</t>
+  </si>
+  <si>
+    <t>MCC [1.2282.0.0] Season 6.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.2241.0.0] Season 6.0</t>
+  </si>
+  <si>
+    <t>MCC [1.2094.0.0] Season 5.0</t>
+  </si>
+  <si>
+    <t>MCC [1.2028.0.0] Season 4.1</t>
+  </si>
+  <si>
+    <t>MCC [1.1955.0.0] Season 4.0</t>
+  </si>
+  <si>
+    <t>MCC [1.1871.0.0] Season 3.0 Hotfix 2</t>
+  </si>
+  <si>
+    <t>MCC [1.1864.0.0] Season 3.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.1829.0.0] Season 3.0</t>
+  </si>
+  <si>
+    <t>MCC [1.1716.0.0] Season 2.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.1698.0.0] Season 2.0</t>
+  </si>
+  <si>
+    <t>MCC [1.1619.0.0] Season 1.2 Hotfix 2</t>
+  </si>
+  <si>
+    <t>MCC [1.1570.0.0] Season 1.2 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.1520.0.0] Season 1.2</t>
+  </si>
+  <si>
+    <t>MCC [1.1389.0.0] Season 1.1 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.1384.0.0] Season 1.1</t>
+  </si>
+  <si>
+    <t>MCC [1.1305.0.0] Season 1.0 Hotfix 2</t>
+  </si>
+  <si>
+    <t>MCC [1.1270.0.0] Season 1.0 Hotfix 1</t>
+  </si>
+  <si>
+    <t>MCC [1.1246.0.0] Season 1.0</t>
   </si>
 </sst>
 </file>
@@ -2807,30 +2915,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84ABB3D-4FC8-48D1-8D8C-D6872D11DBF5}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="136.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="136.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>367</v>
       </c>
@@ -2841,46 +2950,49 @@
         <v>34</v>
       </c>
       <c r="D1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E1" t="s">
         <v>368</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>369</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>370</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>371</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>374</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>375</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>376</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>377</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>378</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>379</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>380</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>372</v>
       </c>
@@ -2888,37 +3000,40 @@
         <v>668</v>
       </c>
       <c r="C2" t="s">
-        <v>709</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2" t="s">
+        <v>765</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
-        <v>707</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" t="s">
+        <v>704</v>
+      </c>
+      <c r="J2" t="s">
         <v>393</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>421</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>456</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>528</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>562</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>372</v>
       </c>
@@ -2926,37 +3041,40 @@
         <v>669</v>
       </c>
       <c r="C3" t="s">
+        <v>801</v>
+      </c>
+      <c r="D3" t="s">
+        <v>766</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
         <v>704</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>707</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>394</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>422</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>457</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>529</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>563</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>372</v>
       </c>
@@ -2964,37 +3082,40 @@
         <v>670</v>
       </c>
       <c r="C4" t="s">
-        <v>708</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="D4" t="s">
+        <v>767</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
-        <v>706</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4" t="s">
+        <v>703</v>
+      </c>
+      <c r="J4" t="s">
         <v>395</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>423</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>458</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>530</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>564</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>372</v>
       </c>
@@ -3002,37 +3123,40 @@
         <v>671</v>
       </c>
       <c r="C5" t="s">
-        <v>710</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="D5" t="s">
+        <v>767</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F5" t="s">
-        <v>705</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G5" t="s">
+        <v>702</v>
+      </c>
+      <c r="J5" t="s">
         <v>396</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>424</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>459</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>531</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>565</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>372</v>
       </c>
@@ -3040,37 +3164,40 @@
         <v>672</v>
       </c>
       <c r="C6" t="s">
+        <v>804</v>
+      </c>
+      <c r="D6" t="s">
+        <v>768</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
         <v>702</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>705</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>397</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>425</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>460</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>532</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>566</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>372</v>
       </c>
@@ -3078,37 +3205,40 @@
         <v>673</v>
       </c>
       <c r="C7" t="s">
-        <v>703</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="D7" t="s">
+        <v>769</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
-        <v>711</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7" t="s">
+        <v>705</v>
+      </c>
+      <c r="J7" t="s">
         <v>398</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>426</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>461</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>533</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>567</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>372</v>
       </c>
@@ -3116,37 +3246,40 @@
         <v>674</v>
       </c>
       <c r="C8" t="s">
-        <v>773</v>
-      </c>
-      <c r="E8" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="D8" t="s">
+        <v>770</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F8" t="s">
-        <v>772</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" t="s">
+        <v>737</v>
+      </c>
+      <c r="J8" t="s">
         <v>399</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>427</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>462</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>534</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>568</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>372</v>
       </c>
@@ -3154,37 +3287,40 @@
         <v>675</v>
       </c>
       <c r="C9" t="s">
+        <v>807</v>
+      </c>
+      <c r="D9" t="s">
         <v>771</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
-        <v>712</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" t="s">
+        <v>706</v>
+      </c>
+      <c r="J9" t="s">
         <v>400</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>428</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>463</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>535</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>569</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>372</v>
       </c>
@@ -3192,37 +3328,40 @@
         <v>676</v>
       </c>
       <c r="C10" t="s">
-        <v>770</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="D10" t="s">
+        <v>772</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F10" t="s">
-        <v>712</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="G10" t="s">
+        <v>706</v>
+      </c>
+      <c r="J10" t="s">
         <v>401</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>429</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>464</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>536</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>570</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>372</v>
       </c>
@@ -3230,37 +3369,40 @@
         <v>677</v>
       </c>
       <c r="C11" t="s">
-        <v>769</v>
-      </c>
-      <c r="E11" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D11" t="s">
+        <v>773</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F11" t="s">
-        <v>712</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G11" t="s">
+        <v>706</v>
+      </c>
+      <c r="J11" t="s">
         <v>402</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>430</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>465</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>537</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>571</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>372</v>
       </c>
@@ -3268,37 +3410,40 @@
         <v>678</v>
       </c>
       <c r="C12" t="s">
-        <v>768</v>
-      </c>
-      <c r="E12" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="D12" t="s">
+        <v>774</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F12" t="s">
-        <v>712</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" t="s">
+        <v>706</v>
+      </c>
+      <c r="J12" t="s">
         <v>403</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>431</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>466</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>538</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>572</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>372</v>
       </c>
@@ -3306,37 +3451,40 @@
         <v>679</v>
       </c>
       <c r="C13" t="s">
-        <v>767</v>
-      </c>
-      <c r="E13" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="D13" t="s">
+        <v>775</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" t="s">
-        <v>766</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G13" t="s">
+        <v>736</v>
+      </c>
+      <c r="J13" t="s">
         <v>404</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>432</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>467</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>539</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>573</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>372</v>
       </c>
@@ -3344,37 +3492,40 @@
         <v>680</v>
       </c>
       <c r="C14" t="s">
-        <v>715</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="D14" t="s">
+        <v>776</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
-        <v>765</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="G14" t="s">
+        <v>735</v>
+      </c>
+      <c r="J14" t="s">
         <v>405</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>433</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>468</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>540</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>574</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>372</v>
       </c>
@@ -3382,37 +3533,40 @@
         <v>681</v>
       </c>
       <c r="C15" t="s">
-        <v>714</v>
-      </c>
-      <c r="E15" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="D15" t="s">
+        <v>777</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F15" t="s">
-        <v>764</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="G15" t="s">
+        <v>734</v>
+      </c>
+      <c r="J15" t="s">
         <v>406</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>434</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>469</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>541</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>575</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>372</v>
       </c>
@@ -3420,37 +3574,40 @@
         <v>682</v>
       </c>
       <c r="C16" t="s">
-        <v>713</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="D16" t="s">
+        <v>778</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
-        <v>763</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="G16" t="s">
+        <v>733</v>
+      </c>
+      <c r="J16" t="s">
         <v>407</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>435</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>470</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>542</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>576</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>372</v>
       </c>
@@ -3458,37 +3615,40 @@
         <v>683</v>
       </c>
       <c r="C17" t="s">
-        <v>762</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="D17" t="s">
+        <v>779</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F17" t="s">
-        <v>760</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="G17" t="s">
+        <v>732</v>
+      </c>
+      <c r="J17" t="s">
         <v>408</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>436</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>471</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>543</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>577</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -3496,37 +3656,40 @@
         <v>684</v>
       </c>
       <c r="C18" t="s">
-        <v>761</v>
-      </c>
-      <c r="E18" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="D18" t="s">
+        <v>780</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F18" t="s">
-        <v>759</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="G18" t="s">
+        <v>731</v>
+      </c>
+      <c r="J18" t="s">
         <v>409</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>437</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>472</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>544</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>578</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>372</v>
       </c>
@@ -3534,37 +3697,40 @@
         <v>685</v>
       </c>
       <c r="C19" t="s">
-        <v>716</v>
-      </c>
-      <c r="E19" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="D19" t="s">
+        <v>781</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F19" t="s">
-        <v>758</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="G19" t="s">
+        <v>730</v>
+      </c>
+      <c r="J19" t="s">
         <v>410</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>438</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>473</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>545</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>579</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>372</v>
       </c>
@@ -3572,37 +3738,40 @@
         <v>686</v>
       </c>
       <c r="C20" t="s">
-        <v>757</v>
-      </c>
-      <c r="E20" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="D20" t="s">
+        <v>782</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F20" t="s">
-        <v>756</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="G20" t="s">
+        <v>729</v>
+      </c>
+      <c r="J20" t="s">
         <v>411</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>439</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>474</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>546</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>580</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>372</v>
       </c>
@@ -3610,37 +3779,40 @@
         <v>687</v>
       </c>
       <c r="C21" t="s">
-        <v>717</v>
-      </c>
-      <c r="E21" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="D21" t="s">
+        <v>783</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F21" t="s">
-        <v>755</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="G21" t="s">
+        <v>728</v>
+      </c>
+      <c r="J21" t="s">
         <v>412</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>440</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>475</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>547</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>581</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>372</v>
       </c>
@@ -3648,37 +3820,40 @@
         <v>688</v>
       </c>
       <c r="C22" t="s">
-        <v>718</v>
-      </c>
-      <c r="E22" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="D22" t="s">
+        <v>784</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F22" t="s">
-        <v>754</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="G22" t="s">
+        <v>727</v>
+      </c>
+      <c r="J22" t="s">
         <v>413</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>441</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>476</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>548</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>582</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>372</v>
       </c>
@@ -3686,37 +3861,40 @@
         <v>689</v>
       </c>
       <c r="C23" t="s">
-        <v>721</v>
-      </c>
-      <c r="E23" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="D23" t="s">
+        <v>785</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F23" t="s">
-        <v>753</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="G23" t="s">
+        <v>726</v>
+      </c>
+      <c r="J23" t="s">
         <v>414</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>442</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>477</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>549</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>583</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>372</v>
       </c>
@@ -3724,40 +3902,43 @@
         <v>690</v>
       </c>
       <c r="C24" t="s">
-        <v>719</v>
-      </c>
-      <c r="E24" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="D24" t="s">
+        <v>786</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F24" t="s">
-        <v>750</v>
-      </c>
       <c r="G24" t="s">
-        <v>744</v>
-      </c>
-      <c r="I24" t="s">
+        <v>724</v>
+      </c>
+      <c r="H24" t="s">
+        <v>720</v>
+      </c>
+      <c r="J24" t="s">
         <v>415</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>443</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>478</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>550</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>584</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>372</v>
       </c>
@@ -3765,34 +3946,37 @@
         <v>691</v>
       </c>
       <c r="C25" t="s">
-        <v>752</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="D25" t="s">
+        <v>787</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F25" t="s">
-        <v>751</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="G25" t="s">
+        <v>725</v>
+      </c>
+      <c r="J25" t="s">
         <v>416</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>444</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>479</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>551</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>372</v>
       </c>
@@ -3800,34 +3984,37 @@
         <v>692</v>
       </c>
       <c r="C26" t="s">
-        <v>749</v>
-      </c>
-      <c r="E26" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="D26" t="s">
+        <v>788</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F26" t="s">
-        <v>748</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="G26" t="s">
+        <v>723</v>
+      </c>
+      <c r="J26" t="s">
         <v>417</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>445</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>480</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>552</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>372</v>
       </c>
@@ -3835,37 +4022,40 @@
         <v>693</v>
       </c>
       <c r="C27" t="s">
+        <v>825</v>
+      </c>
+      <c r="D27" t="s">
+        <v>789</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
         <v>722</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" t="s">
-        <v>747</v>
-      </c>
-      <c r="G27" t="s">
-        <v>743</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="H27" t="s">
+        <v>719</v>
+      </c>
+      <c r="J27" t="s">
         <v>384</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>446</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>481</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>553</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>372</v>
       </c>
@@ -3873,31 +4063,34 @@
         <v>694</v>
       </c>
       <c r="C28" t="s">
-        <v>746</v>
-      </c>
-      <c r="E28" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="D28" t="s">
+        <v>790</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F28" t="s">
-        <v>745</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="G28" t="s">
+        <v>721</v>
+      </c>
+      <c r="J28" t="s">
         <v>385</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>447</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>482</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>372</v>
       </c>
@@ -3905,34 +4098,37 @@
         <v>695</v>
       </c>
       <c r="C29" t="s">
-        <v>723</v>
-      </c>
-      <c r="E29" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="D29" t="s">
+        <v>791</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F29" t="s">
-        <v>741</v>
-      </c>
       <c r="G29" t="s">
-        <v>742</v>
-      </c>
-      <c r="I29" t="s">
+        <v>717</v>
+      </c>
+      <c r="H29" t="s">
+        <v>718</v>
+      </c>
+      <c r="J29" t="s">
         <v>386</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>448</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>483</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>372</v>
       </c>
@@ -3940,28 +4136,31 @@
         <v>696</v>
       </c>
       <c r="C30" t="s">
-        <v>740</v>
-      </c>
-      <c r="E30" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="D30" t="s">
+        <v>792</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F30" t="s">
-        <v>739</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="G30" t="s">
+        <v>716</v>
+      </c>
+      <c r="J30" t="s">
         <v>387</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>449</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>484</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>372</v>
       </c>
@@ -3969,28 +4168,31 @@
         <v>697</v>
       </c>
       <c r="C31" t="s">
-        <v>737</v>
-      </c>
-      <c r="E31" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="D31" t="s">
+        <v>793</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F31" t="s">
-        <v>738</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="G31" t="s">
+        <v>715</v>
+      </c>
+      <c r="J31" t="s">
         <v>388</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>450</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>485</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>372</v>
       </c>
@@ -3998,31 +4200,34 @@
         <v>698</v>
       </c>
       <c r="C32" t="s">
-        <v>736</v>
-      </c>
-      <c r="E32" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="D32" t="s">
+        <v>794</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F32" t="s">
-        <v>734</v>
-      </c>
       <c r="G32" t="s">
-        <v>735</v>
-      </c>
-      <c r="I32" t="s">
+        <v>713</v>
+      </c>
+      <c r="H32" t="s">
+        <v>714</v>
+      </c>
+      <c r="J32" t="s">
         <v>389</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>451</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>486</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>372</v>
       </c>
@@ -4030,25 +4235,28 @@
         <v>699</v>
       </c>
       <c r="C33" t="s">
-        <v>733</v>
-      </c>
-      <c r="E33" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="D33" t="s">
+        <v>795</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F33" t="s">
-        <v>730</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="G33" t="s">
+        <v>710</v>
+      </c>
+      <c r="J33" t="s">
         <v>390</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>452</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>372</v>
       </c>
@@ -4056,28 +4264,31 @@
         <v>700</v>
       </c>
       <c r="C34" t="s">
-        <v>720</v>
-      </c>
-      <c r="E34" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="D34" t="s">
+        <v>796</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F34" t="s">
-        <v>729</v>
-      </c>
       <c r="G34" t="s">
-        <v>731</v>
-      </c>
-      <c r="I34" t="s">
+        <v>709</v>
+      </c>
+      <c r="H34" t="s">
+        <v>711</v>
+      </c>
+      <c r="J34" t="s">
         <v>391</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>453</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>372</v>
       </c>
@@ -4085,22 +4296,25 @@
         <v>701</v>
       </c>
       <c r="C35" t="s">
-        <v>728</v>
-      </c>
-      <c r="E35" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="D35" t="s">
+        <v>797</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F35" t="s">
-        <v>726</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="G35" t="s">
+        <v>708</v>
+      </c>
+      <c r="J35" t="s">
         <v>392</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>372</v>
       </c>
@@ -4108,22 +4322,25 @@
         <v>667</v>
       </c>
       <c r="C36" t="s">
-        <v>727</v>
-      </c>
-      <c r="E36" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="D36" t="s">
+        <v>798</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F36" t="s">
-        <v>725</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="G36" t="s">
+        <v>707</v>
+      </c>
+      <c r="J36" t="s">
         <v>382</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>372</v>
       </c>
@@ -4131,25 +4348,28 @@
         <v>666</v>
       </c>
       <c r="C37" t="s">
-        <v>724</v>
-      </c>
-      <c r="E37" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="D37" t="s">
+        <v>799</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F37" t="s">
-        <v>774</v>
-      </c>
       <c r="G37" t="s">
-        <v>732</v>
-      </c>
-      <c r="I37" t="s">
+        <v>738</v>
+      </c>
+      <c r="H37" t="s">
+        <v>712</v>
+      </c>
+      <c r="J37" t="s">
         <v>383</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>660</v>
       </c>
@@ -4157,16 +4377,16 @@
         <v>652</v>
       </c>
       <c r="C38" t="s">
-        <v>777</v>
-      </c>
-      <c r="E38" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>660</v>
       </c>
@@ -4174,16 +4394,16 @@
         <v>653</v>
       </c>
       <c r="C39" t="s">
-        <v>778</v>
-      </c>
-      <c r="E39" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>660</v>
       </c>
@@ -4191,16 +4411,16 @@
         <v>630</v>
       </c>
       <c r="C40" t="s">
-        <v>779</v>
-      </c>
-      <c r="E40" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>660</v>
       </c>
@@ -4208,16 +4428,16 @@
         <v>631</v>
       </c>
       <c r="C41" t="s">
-        <v>780</v>
-      </c>
-      <c r="E41" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>660</v>
       </c>
@@ -4225,16 +4445,16 @@
         <v>632</v>
       </c>
       <c r="C42" t="s">
-        <v>781</v>
-      </c>
-      <c r="E42" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>660</v>
       </c>
@@ -4242,16 +4462,16 @@
         <v>633</v>
       </c>
       <c r="C43" t="s">
-        <v>782</v>
-      </c>
-      <c r="E43" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>660</v>
       </c>
@@ -4259,16 +4479,16 @@
         <v>634</v>
       </c>
       <c r="C44" t="s">
-        <v>783</v>
-      </c>
-      <c r="E44" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>660</v>
       </c>
@@ -4276,16 +4496,16 @@
         <v>635</v>
       </c>
       <c r="C45" t="s">
-        <v>784</v>
-      </c>
-      <c r="E45" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>660</v>
       </c>
@@ -4293,16 +4513,16 @@
         <v>636</v>
       </c>
       <c r="C46" t="s">
-        <v>785</v>
-      </c>
-      <c r="E46" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>660</v>
       </c>
@@ -4310,16 +4530,16 @@
         <v>637</v>
       </c>
       <c r="C47" t="s">
-        <v>786</v>
-      </c>
-      <c r="E47" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>660</v>
       </c>
@@ -4327,16 +4547,16 @@
         <v>638</v>
       </c>
       <c r="C48" t="s">
-        <v>787</v>
-      </c>
-      <c r="E48" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>660</v>
       </c>
@@ -4344,16 +4564,16 @@
         <v>639</v>
       </c>
       <c r="C49" t="s">
-        <v>788</v>
-      </c>
-      <c r="E49" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>660</v>
       </c>
@@ -4361,16 +4581,16 @@
         <v>640</v>
       </c>
       <c r="C50" t="s">
-        <v>789</v>
-      </c>
-      <c r="E50" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>660</v>
       </c>
@@ -4378,16 +4598,16 @@
         <v>641</v>
       </c>
       <c r="C51" t="s">
-        <v>790</v>
-      </c>
-      <c r="E51" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>660</v>
       </c>
@@ -4395,16 +4615,16 @@
         <v>642</v>
       </c>
       <c r="C52" t="s">
-        <v>791</v>
-      </c>
-      <c r="E52" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>660</v>
       </c>
@@ -4412,16 +4632,16 @@
         <v>643</v>
       </c>
       <c r="C53" t="s">
-        <v>792</v>
-      </c>
-      <c r="E53" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>660</v>
       </c>
@@ -4429,16 +4649,16 @@
         <v>644</v>
       </c>
       <c r="C54" t="s">
-        <v>793</v>
-      </c>
-      <c r="E54" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>660</v>
       </c>
@@ -4446,16 +4666,16 @@
         <v>645</v>
       </c>
       <c r="C55" t="s">
-        <v>794</v>
-      </c>
-      <c r="E55" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>660</v>
       </c>
@@ -4463,16 +4683,16 @@
         <v>646</v>
       </c>
       <c r="C56" t="s">
-        <v>795</v>
-      </c>
-      <c r="E56" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>660</v>
       </c>
@@ -4480,16 +4700,16 @@
         <v>647</v>
       </c>
       <c r="C57" t="s">
-        <v>796</v>
-      </c>
-      <c r="E57" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>660</v>
       </c>
@@ -4497,16 +4717,16 @@
         <v>648</v>
       </c>
       <c r="C58" t="s">
-        <v>797</v>
-      </c>
-      <c r="E58" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>660</v>
       </c>
@@ -4514,16 +4734,16 @@
         <v>649</v>
       </c>
       <c r="C59" t="s">
-        <v>798</v>
-      </c>
-      <c r="E59" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>660</v>
       </c>
@@ -4531,16 +4751,16 @@
         <v>650</v>
       </c>
       <c r="C60" t="s">
-        <v>799</v>
-      </c>
-      <c r="E60" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>660</v>
       </c>
@@ -4548,16 +4768,16 @@
         <v>651</v>
       </c>
       <c r="C61" t="s">
-        <v>776</v>
-      </c>
-      <c r="E61" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>660</v>
       </c>
@@ -4565,12 +4785,12 @@
         <v>629</v>
       </c>
       <c r="C62" t="s">
-        <v>775</v>
-      </c>
-      <c r="E62" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>629</v>
       </c>
     </row>

</xml_diff>